<commit_message>
updated a-d conector pins
</commit_message>
<xml_diff>
--- a/Hardware/Main Board V1.2/BOM LCSC.xlsx
+++ b/Hardware/Main Board V1.2/BOM LCSC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Main Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Main Board V1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52165D3-78CD-4B9A-92D7-9BB6C2C6CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481BFF43-B8AA-4A1E-B4E0-20682ED3DBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42330" yWindow="5340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -3275,8 +3275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
   <dimension ref="B1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N18" s="19"/>
       <c r="O18" s="17"/>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N19" s="19"/>
       <c r="O19" s="17"/>
@@ -4785,7 +4785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E6E9A4-984E-47E0-AB78-3A5B51A2C28B}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>